<commit_message>
ref alternative porte fuse, Théo le zozo va procéder à des mesures de grande importance
</commit_message>
<xml_diff>
--- a/HW/sourcing.xlsx
+++ b/HW/sourcing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Softcar-ELEC\Documents\Git\LED-PCB-V1\HW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EFD8F31-F038-4720-AE4A-FAE999068FDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73568265-2200-461B-B00A-88C4F9DC1077}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="57">
   <si>
     <t>Reference</t>
   </si>
@@ -196,6 +196,12 @@
   </si>
   <si>
     <t>EMZS250ARA102MJA0G</t>
+  </si>
+  <si>
+    <t>Diamètre à définir</t>
+  </si>
+  <si>
+    <t>BK1/HTC-100M</t>
   </si>
 </sst>
 </file>
@@ -728,7 +734,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1089,7 +1095,7 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1329,8 +1335,12 @@
       <c r="F9" s="1">
         <v>0.76700000000000002</v>
       </c>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
+      <c r="G9" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0.72199999999999998</v>
+      </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
     </row>
@@ -1396,7 +1406,9 @@
       <c r="F12" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G12" s="1"/>
+      <c r="G12" s="1" t="s">
+        <v>55</v>
+      </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>

</xml_diff>

<commit_message>
Ajout ref connecteur alim
</commit_message>
<xml_diff>
--- a/HW/sourcing.xlsx
+++ b/HW/sourcing.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Softcar-ELEC\Documents\Git\LED-PCB-V1\HW\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jvien\Documents\Git\LED-PCB-V1\HW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73568265-2200-461B-B00A-88C4F9DC1077}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DD92E50-52E3-4E65-9D02-C6C98479D606}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sourcing" sheetId="1" r:id="rId1"/>
@@ -198,10 +198,10 @@
     <t>EMZS250ARA102MJA0G</t>
   </si>
   <si>
-    <t>Diamètre à définir</t>
-  </si>
-  <si>
     <t>BK1/HTC-100M</t>
+  </si>
+  <si>
+    <t>694106301002</t>
   </si>
 </sst>
 </file>
@@ -719,7 +719,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -735,6 +735,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1094,24 +1097,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="51" customWidth="1"/>
-    <col min="3" max="3" width="25.140625" customWidth="1"/>
-    <col min="4" max="4" width="41.140625" customWidth="1"/>
-    <col min="5" max="5" width="25.85546875" customWidth="1"/>
+    <col min="3" max="3" width="25.109375" customWidth="1"/>
+    <col min="4" max="4" width="41.109375" customWidth="1"/>
+    <col min="5" max="5" width="25.88671875" customWidth="1"/>
     <col min="6" max="6" width="10" customWidth="1"/>
-    <col min="7" max="7" width="32.28515625" customWidth="1"/>
+    <col min="7" max="7" width="32.33203125" customWidth="1"/>
     <col min="8" max="8" width="10" customWidth="1"/>
-    <col min="9" max="9" width="30.140625" customWidth="1"/>
+    <col min="9" max="9" width="30.109375" customWidth="1"/>
     <col min="10" max="10" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1143,7 +1146,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>51</v>
       </c>
@@ -1167,7 +1170,7 @@
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>50</v>
       </c>
@@ -1192,7 +1195,7 @@
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
@@ -1215,7 +1218,7 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
@@ -1243,7 +1246,7 @@
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
@@ -1266,7 +1269,7 @@
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>22</v>
       </c>
@@ -1288,7 +1291,7 @@
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
@@ -1318,7 +1321,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>41</v>
       </c>
@@ -1336,7 +1339,7 @@
         <v>0.76700000000000002</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H9" s="1">
         <v>0.72199999999999998</v>
@@ -1344,7 +1347,7 @@
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>27</v>
       </c>
@@ -1366,7 +1369,7 @@
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>29</v>
       </c>
@@ -1389,7 +1392,7 @@
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>32</v>
       </c>
@@ -1406,14 +1409,16 @@
       <c r="F12" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G12" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="H12" s="1"/>
+      <c r="G12" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="H12" s="1">
+        <v>0.92100000000000004</v>
+      </c>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>36</v>
       </c>
@@ -1435,24 +1440,24 @@
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F14">
         <f>SUM(F2:F13)</f>
         <v>14.286</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>10</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="290" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="290" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>